<commit_message>
27-03-2023 -> Regretion DPLKINV001-001 until DPLKINV025-001, DPLKKEU001-001 until DPLKKEU005-001
28-03-2023
-> Regretion DPLKINV026-001 until DPLKINV090-001

29-03-2023
-> Regretion DPLKINV091-001 until DPLKINV125-001, DPLKINV144-001 until DPLKINV146-001, DPLKKPS001-001 until DPLKKPS096

30-03-2023
-> Regretion DPLKINV138-001, DPLKKPS123-001, DPLKKPS124-001, DPLKKPS130-001, DPLKKPS135-001 until DPLKKPS140-001, DPLKKPS149-001, DPLKKPS149-002, DPLKKPS152-001 until DPLKKPS153-002

31-03-2023
-> Regretion DPLKKEU007-001, DPLKKEU008-001, DPLKKEU012-001, DPLKKEU029-001, DPLKKEU031-001, DPLKKEU039-001, DPLKKEU041-001, DPLKKEU042-001, DPLKKEU045-001, DPLKKPS122-001, DPLKKPS128-001, DPLKKPS143-001 until DPLKKPS144-002, DPLKKPS150-001, DPLKKPS150-002
</commit_message>
<xml_diff>
--- a/DPLKKPS135-001 - Kepesertaan - Transaksi - Register Perjanjian Kerja Sama - Pending Register/Report/Report/Default.xlsx
+++ b/DPLKKPS135-001 - Kepesertaan - Transaksi - Register Perjanjian Kerja Sama - Pending Register/Report/Report/Default.xlsx
@@ -8,7 +8,7 @@
   </bookViews>
   <sheets>
     <sheet name="Global" sheetId="1" r:id="rId1"/>
-    <sheet name="DPLKINV003-001-Investasi-Fixed" sheetId="2" r:id="rId2"/>
+    <sheet name="KPS135-001-RegisterPKS" sheetId="2" r:id="rId2"/>
     <sheet name="TEMPORARY" sheetId="3" r:id="rId3"/>
     <sheet name="DPLKDBConfig" sheetId="4" r:id="rId4"/>
   </sheets>
@@ -17,7 +17,10 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="118">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="137">
+  <si>
+    <t>URL_ICONS</t>
+  </si>
   <si>
     <t>PROJECT_NAME</t>
   </si>
@@ -28,7 +31,13 @@
     <t>PROGRAM_PATH2</t>
   </si>
   <si>
-    <t>TANGGAL_MARKET</t>
+    <t>Kepesertaan</t>
+  </si>
+  <si>
+    <t>PRD0002</t>
+  </si>
+  <si>
+    <t>http://192.168.150.186/alternity/</t>
   </si>
   <si>
     <t>PROGRAM3</t>
@@ -37,15 +46,9 @@
     <t>C:\Program Files\HeidiSQL</t>
   </si>
   <si>
-    <t>DPLKINV003-001</t>
-  </si>
-  <si>
     <t>VALUTA</t>
   </si>
   <si>
-    <t>FILE_EXCEL</t>
-  </si>
-  <si>
     <t>AD</t>
   </si>
   <si>
@@ -64,24 +67,27 @@
     <t>RUN</t>
   </si>
   <si>
-    <t>IDR : Rupiah</t>
+    <t>ROLE</t>
+  </si>
+  <si>
+    <t>Asisten Settlement</t>
   </si>
   <si>
     <t>R</t>
   </si>
   <si>
+    <t>PASSWORD_DB</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY1</t>
+  </si>
+  <si>
+    <t>N</t>
+  </si>
+  <si>
     <t>V</t>
   </si>
   <si>
-    <t>PASSWORD_DB</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY1</t>
-  </si>
-  <si>
-    <t>N</t>
-  </si>
-  <si>
     <t>AP</t>
   </si>
   <si>
@@ -100,12 +106,6 @@
     <t>USERID</t>
   </si>
   <si>
-    <t>Fixed Income</t>
-  </si>
-  <si>
-    <t>01012023HargaPasarFixedIncome.xlsx</t>
-  </si>
-  <si>
     <t>QUERY_SETUP_PORTOFOLIO</t>
   </si>
   <si>
@@ -118,12 +118,21 @@
     <t>PROGRAM_PATH3</t>
   </si>
   <si>
-    <t>Normal - Investasi - Upload Harga Pasar</t>
-  </si>
-  <si>
     <t>SIDEBAR_MENU</t>
   </si>
   <si>
+    <t>SIDEBAR_SUBMENU_SUBMENU</t>
+  </si>
+  <si>
+    <t>NO_PKS</t>
+  </si>
+  <si>
+    <t>JENIS_DOKUMEN_PERJANJIAN</t>
+  </si>
+  <si>
+    <t>NO_KOLEKTIF</t>
+  </si>
+  <si>
     <t>QUERY2</t>
   </si>
   <si>
@@ -136,6 +145,18 @@
     <t>Automation Test Execution Document</t>
   </si>
   <si>
+    <t>K</t>
+  </si>
+  <si>
+    <t>PPIP</t>
+  </si>
+  <si>
+    <t>KEP-009</t>
+  </si>
+  <si>
+    <t>TGL_BERAKHIR</t>
+  </si>
+  <si>
     <t>USER_DB</t>
   </si>
   <si>
@@ -151,85 +172,120 @@
     <t>TESTER2</t>
   </si>
   <si>
-    <t>Username : 32382;
+    <t>JENIS_PERJANJIAN</t>
+  </si>
+  <si>
+    <t>STATUS_REGISTER</t>
+  </si>
+  <si>
+    <t>EXPL_QUERY2</t>
+  </si>
+  <si>
+    <t>O</t>
+  </si>
+  <si>
+    <t>S</t>
+  </si>
+  <si>
+    <t>AM</t>
+  </si>
+  <si>
+    <t>AQ</t>
+  </si>
+  <si>
+    <t>BROWSER_VERSION</t>
+  </si>
+  <si>
+    <t>COVER_TITLE</t>
+  </si>
+  <si>
+    <t>Regression Test</t>
+  </si>
+  <si>
+    <t>DEVELOPMENT_MANAGER</t>
+  </si>
+  <si>
+    <t>Proses Register Berhasil dan data masuk ke list register</t>
+  </si>
+  <si>
+    <t>Transaksi</t>
+  </si>
+  <si>
+    <t>KEPESERTAAN</t>
+  </si>
+  <si>
+    <t>W</t>
+  </si>
+  <si>
+    <t>107.0.5304.107 (Official Build) (64-bit)</t>
+  </si>
+  <si>
+    <t>BROWSER_ICONS</t>
+  </si>
+  <si>
+    <t>filezilla</t>
+  </si>
+  <si>
+    <t>PREPARATION</t>
+  </si>
+  <si>
+    <t>MAIN_SIDEBAR</t>
+  </si>
+  <si>
+    <t>000008578</t>
+  </si>
+  <si>
+    <t>TGL_MULAI</t>
+  </si>
+  <si>
+    <t>sa</t>
+  </si>
+  <si>
+    <t>select * from dbo.inv_ms_portofolio where porto_id = '&lt;OBJECT_1&gt;';</t>
+  </si>
+  <si>
+    <t>DATABASE_2</t>
+  </si>
+  <si>
+    <t>AB</t>
+  </si>
+  <si>
+    <t>AUTHOR</t>
+  </si>
+  <si>
+    <t>Automation Team</t>
+  </si>
+  <si>
+    <t>TESTING_GROUPHEAD</t>
+  </si>
+  <si>
+    <t>PROGRAM1</t>
+  </si>
+  <si>
+    <t>DPLKKPS135-001</t>
+  </si>
+  <si>
+    <t>Normal - Kepesertaan - Transaksi</t>
+  </si>
+  <si>
+    <t>Username : 30603;
 Password : bni1234;
-Tgl. Market : 01/01/2023;
-File Excel : 01012023HargaPasarFixedIncome.xlsx</t>
-  </si>
-  <si>
-    <t>O</t>
-  </si>
-  <si>
-    <t>S</t>
-  </si>
-  <si>
-    <t>EXPL_QUERY2</t>
-  </si>
-  <si>
-    <t>AM</t>
-  </si>
-  <si>
-    <t>AQ</t>
-  </si>
-  <si>
-    <t>BROWSER_VERSION</t>
-  </si>
-  <si>
-    <t>COVER_TITLE</t>
-  </si>
-  <si>
-    <t>Regression Test</t>
-  </si>
-  <si>
-    <t>DEVELOPMENT_MANAGER</t>
-  </si>
-  <si>
-    <t>Investasi</t>
-  </si>
-  <si>
-    <t>W</t>
-  </si>
-  <si>
-    <t>107.0.5304.107 (Official Build) (64-bit)</t>
-  </si>
-  <si>
-    <t>BROWSER_ICONS</t>
-  </si>
-  <si>
-    <t>filezilla</t>
-  </si>
-  <si>
-    <t>Upload harga pasar Reksadana - Fixed Income dapat dilakukan dengan baik</t>
-  </si>
-  <si>
-    <t>PREPARATION</t>
-  </si>
-  <si>
-    <t>MAIN_SIDEBAR</t>
-  </si>
-  <si>
-    <t>sa</t>
-  </si>
-  <si>
-    <t>select * from dbo.inv_ms_portofolio where porto_id = '&lt;OBJECT_1&gt;';</t>
-  </si>
-  <si>
-    <t>DATABASE_2</t>
-  </si>
-  <si>
-    <t>AB</t>
-  </si>
-  <si>
-    <t>AUTHOR</t>
-  </si>
-  <si>
-    <t>Automation Team</t>
-  </si>
-  <si>
-    <t>TESTING_GROUPHEAD</t>
-  </si>
-  <si>
-    <t>PROGRAM1</t>
+Role : 10 - Asisten Settlement;
+No PKS : 82329788;
+Jenis Dokumen Perjanjian : 1 : PKS;
+Jenis Perjanjian : K : Konvensional;
+No Kolektif : 000002390;
+Kepesertaan : PRD0002 : Kepesertaan Kolektif;
+Jenis Program Pensiun : PPIP : Program Pensiun Iuran Pasti;
+Keterangan : KEP-009;
+Valuta : R : Rupiah;
+Tanggal Mulai : 01/01/2022;
+Tanggal Berakhir : 01/01/2032;
+Status Register : 0 : Pending Register
+Keterangan : KEP-009</t>
+  </si>
+  <si>
+    <t>Register Perjanjian Kerja Sama</t>
   </si>
   <si>
     <t>QUERY3</t>
@@ -259,7 +315,7 @@
     <t>TC_ID</t>
   </si>
   <si>
-    <t>Investasi - Fixed Income</t>
+    <t>EXPL_QUERY3</t>
   </si>
   <si>
     <t>P</t>
@@ -268,9 +324,6 @@
     <t>T</t>
   </si>
   <si>
-    <t>EXPL_QUERY3</t>
-  </si>
-  <si>
     <t>AN</t>
   </si>
   <si>
@@ -286,7 +339,7 @@
     <t>PROGRAM_PATH1</t>
   </si>
   <si>
-    <t>Entry Harga Pasar</t>
+    <t>KETERANGAN</t>
   </si>
   <si>
     <t>X</t>
@@ -319,6 +372,9 @@
     <t>EXPECTED_RESULT</t>
   </si>
   <si>
+    <t>Perjanjian Kerja Sama</t>
+  </si>
+  <si>
     <t>M</t>
   </si>
   <si>
@@ -340,18 +396,24 @@
     <t>TEST_MANAGER</t>
   </si>
   <si>
+    <t>Register Perjanjian Kerja Sama - Pending Register</t>
+  </si>
+  <si>
     <t>bni1234</t>
   </si>
   <si>
+    <t>KEP-009 Pending Register</t>
+  </si>
+  <si>
+    <t>BNI46sql</t>
+  </si>
+  <si>
     <t>Q</t>
   </si>
   <si>
     <t>U</t>
   </si>
   <si>
-    <t>BNI46sql</t>
-  </si>
-  <si>
     <t>AO</t>
   </si>
   <si>
@@ -368,6 +430,12 @@
   </si>
   <si>
     <t>PASSWORD</t>
+  </si>
+  <si>
+    <t>JENIS_PROGRAM_PENSIUN</t>
+  </si>
+  <si>
+    <t>KETERANGAN_REGISTER</t>
   </si>
   <si>
     <t>HOSTNAME</t>
@@ -398,17 +466,29 @@
       <scheme val="minor"/>
     </font>
     <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <sz val="11"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <sz val="10"/>
       <color rgb="FF000000"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
+      <name val="Arial"/>
+      <family val="2"/>
     </font>
     <font>
       <sz val="11"/>
@@ -417,18 +497,6 @@
       <family val="2"/>
     </font>
     <font>
-      <sz val="10"/>
-      <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
-      <color theme="1"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
       <sz val="11"/>
       <color theme="0"/>
       <name val="Calibri"/>
@@ -439,22 +507,6 @@
       <b/>
       <sz val="11"/>
       <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="13"/>
-      <color theme="3"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <b/>
-      <sz val="11"/>
-      <color rgb="FFFA7D00"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -504,6 +556,29 @@
       <scheme val="major"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color rgb="FFFA7D00"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="13"/>
+      <color theme="3"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
       <b/>
       <sz val="11"/>
       <color rgb="FF3F3F3F"/>
@@ -528,7 +603,7 @@
     </font>
     <font>
       <sz val="11"/>
-      <color rgb="FFFF0000"/>
+      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -537,13 +612,6 @@
       <b/>
       <sz val="11"/>
       <color theme="0"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <sz val="11"/>
-      <color rgb="FF3F3F76"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -594,7 +662,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="26">
+  <cellXfs count="31">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment vertical="center"/>
@@ -607,23 +675,38 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -633,19 +716,51 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="14" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+      <protection locked="0"/>
+    </xf>
+    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="left" vertical="center"/>
+      <protection locked="0"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="1" applyFill="1" applyBorder="1" applyProtection="1">
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
       <protection locked="0"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
@@ -656,39 +771,12 @@
       <alignment vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
       <alignment horizontal="left" vertical="center"/>
       <protection locked="0"/>
     </xf>
-    <xf numFmtId="14" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyProtection="1">
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" quotePrefix="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment vertical="center"/>
-      <protection locked="0"/>
-    </xf>
-    <xf numFmtId="3" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1" applyProtection="1">
-      <alignment horizontal="left" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1" applyProtection="1">
+      <alignment horizontal="center" vertical="center"/>
       <protection locked="0"/>
     </xf>
   </cellXfs>
@@ -988,187 +1076,195 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:Z2"/>
+  <dimension ref="A1:AA2"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView topLeftCell="H1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="13.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="13.28515625" style="10" customWidth="1"/>
-    <col min="3" max="3" width="33.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="25.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="16.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="35.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="13.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="14.5703125" style="10" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="15.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="14" max="15" width="19.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="15.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="20.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="24.28515625" style="10" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="24.7109375" style="10" bestFit="1" customWidth="1"/>
-    <col min="21" max="23" width="11.140625" style="10" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="24.85546875" style="10" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="36.42578125" style="10" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="17" style="10" bestFit="1" customWidth="1"/>
-    <col min="27" max="16384" width="9.078125" style="10" customWidth="1"/>
+    <col min="1" max="1" width="13.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="13.28515625" style="14" customWidth="1"/>
+    <col min="3" max="3" width="33.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="22" style="14" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="30.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="16.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="35.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="13.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="24.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="14.5703125" style="14" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="15.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="15" max="16" width="19.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="15.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="20.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="24.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="24.28515625" style="14" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="24.7109375" style="14" bestFit="1" customWidth="1"/>
+    <col min="22" max="24" width="11.140625" style="14" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="24.85546875" style="14" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="36.42578125" style="14" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="17" style="14" bestFit="1" customWidth="1"/>
+    <col min="28" max="16384" width="9.078125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
       <c r="A1" t="s">
-        <v>102</v>
+        <v>117</v>
       </c>
       <c r="B1" t="s">
-        <v>85</v>
+        <v>99</v>
       </c>
       <c r="C1" t="s">
-        <v>50</v>
+        <v>58</v>
       </c>
       <c r="D1" t="s">
-        <v>103</v>
+        <v>118</v>
       </c>
       <c r="E1" t="s">
-        <v>57</v>
+        <v>0</v>
       </c>
       <c r="F1" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="G1" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="H1" t="s">
+        <v>100</v>
+      </c>
+      <c r="I1" t="s">
         <v>31</v>
       </c>
-      <c r="I1" t="s">
-        <v>113</v>
-      </c>
       <c r="J1" t="s">
-        <v>0</v>
+        <v>130</v>
       </c>
       <c r="K1" t="s">
         <v>1</v>
       </c>
       <c r="L1" t="s">
-        <v>51</v>
+        <v>2</v>
       </c>
       <c r="M1" t="s">
-        <v>114</v>
+        <v>59</v>
       </c>
       <c r="N1" t="s">
-        <v>13</v>
+        <v>131</v>
       </c>
       <c r="O1" t="s">
-        <v>43</v>
+        <v>14</v>
       </c>
       <c r="P1" t="s">
-        <v>105</v>
+        <v>50</v>
       </c>
       <c r="Q1" t="s">
-        <v>68</v>
+        <v>120</v>
       </c>
       <c r="R1" t="s">
-        <v>53</v>
+        <v>79</v>
       </c>
       <c r="S1" t="s">
-        <v>76</v>
+        <v>61</v>
       </c>
       <c r="T1" t="s">
-        <v>24</v>
+        <v>91</v>
       </c>
       <c r="U1" t="s">
-        <v>69</v>
+        <v>26</v>
       </c>
       <c r="V1" t="s">
-        <v>97</v>
+        <v>80</v>
       </c>
       <c r="W1" t="s">
-        <v>4</v>
+        <v>111</v>
       </c>
       <c r="X1" t="s">
-        <v>87</v>
+        <v>7</v>
       </c>
       <c r="Y1" t="s">
-        <v>2</v>
+        <v>101</v>
       </c>
       <c r="Z1" t="s">
+        <v>3</v>
+      </c>
+      <c r="AA1" t="s">
         <v>32</v>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="3" t="s">
-        <v>112</v>
+        <v>129</v>
       </c>
       <c r="B2" s="3" t="s">
-        <v>42</v>
+        <v>49</v>
       </c>
       <c r="C2" s="3" t="s">
-        <v>56</v>
-      </c>
-      <c r="D2" s="14" t="s">
-        <v>74</v>
-      </c>
-      <c r="E2" s="3" t="s">
-        <v>95</v>
-      </c>
-      <c r="F2" s="6" t="s">
-        <v>67</v>
-      </c>
-      <c r="G2" s="6" t="s">
-        <v>38</v>
-      </c>
-      <c r="H2" s="3"/>
-      <c r="I2" s="3" t="s">
-        <v>12</v>
-      </c>
-      <c r="J2" s="6" t="s">
-        <v>96</v>
-      </c>
-      <c r="K2" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D2" s="11" t="s">
+        <v>89</v>
+      </c>
+      <c r="E2" s="11" t="s">
+        <v>6</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="G2" s="5" t="s">
+        <v>78</v>
+      </c>
+      <c r="H2" s="5" t="s">
+        <v>41</v>
+      </c>
+      <c r="I2" s="3"/>
+      <c r="J2" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="K2" s="5" t="s">
+        <v>110</v>
+      </c>
+      <c r="L2" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="M2" s="3" t="s">
+        <v>25</v>
+      </c>
+      <c r="N2" s="3" t="s">
+        <v>60</v>
+      </c>
+      <c r="O2" s="5" t="s">
         <v>90</v>
       </c>
-      <c r="L2" s="3" t="s">
-        <v>23</v>
-      </c>
-      <c r="M2" s="3" t="s">
-        <v>52</v>
-      </c>
-      <c r="N2" s="6" t="s">
-        <v>75</v>
-      </c>
-      <c r="O2" s="6" t="s">
-        <v>104</v>
-      </c>
-      <c r="P2" s="3"/>
+      <c r="P2" s="5" t="s">
+        <v>119</v>
+      </c>
       <c r="Q2" s="3"/>
       <c r="R2" s="3"/>
       <c r="S2" s="3"/>
       <c r="T2" s="3"/>
-      <c r="U2" s="3" t="s">
-        <v>91</v>
-      </c>
+      <c r="U2" s="3"/>
       <c r="V2" s="3" t="s">
-        <v>58</v>
-      </c>
-      <c r="W2" s="3"/>
-      <c r="X2" s="3" t="s">
-        <v>5</v>
-      </c>
+        <v>105</v>
+      </c>
+      <c r="W2" s="3" t="s">
+        <v>68</v>
+      </c>
+      <c r="X2" s="3"/>
       <c r="Y2" s="3" t="s">
-        <v>77</v>
-      </c>
-      <c r="Z2" s="21"/>
+        <v>8</v>
+      </c>
+      <c r="Z2" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="AA2" s="26"/>
     </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="D2" r:id="rId1"/>
+    <hyperlink ref="E2" r:id="rId2"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait"/>
@@ -1177,278 +1273,248 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
-  <dimension ref="A1:V7"/>
+  <dimension ref="A1:Y4"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" workbookViewId="0">
-      <selection activeCell="F2" sqref="F2"/>
+    <sheetView topLeftCell="M1" workbookViewId="0">
+      <selection activeCell="A4" sqref="A4:Y4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="36.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="22.7109375" style="11" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="29.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="32.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" style="11" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="14.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="10" max="10" width="15" style="11" bestFit="1" customWidth="1"/>
-    <col min="11" max="11" width="18.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="11.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="18" style="11" bestFit="1" customWidth="1"/>
-    <col min="14" max="14" width="35" style="11" bestFit="1" customWidth="1"/>
-    <col min="15" max="15" width="10" style="11" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="6.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="9.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="13.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="19" max="19" width="14.42578125" style="11" bestFit="1" customWidth="1"/>
-    <col min="20" max="20" width="13.140625" style="11" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="16.85546875" style="11" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="22.5703125" style="11" bestFit="1" customWidth="1"/>
-    <col min="23" max="16384" width="9.078125" style="11" customWidth="1"/>
+    <col min="1" max="1" width="4.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="27.7109375" style="30" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="20.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="28" style="25" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="32.28515625" style="25" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="6.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="9.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="9.078125" style="25" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.5703125" style="25" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="13.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="18.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="25.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="14" max="14" width="9" style="25" bestFit="1" customWidth="1"/>
+    <col min="15" max="15" width="24.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="14.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="17" max="18" width="11.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="19" max="19" width="21.85546875" style="25" bestFit="1" customWidth="1"/>
+    <col min="20" max="20" width="11" style="25" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="6.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="10.42578125" style="25" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="12.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="14.7109375" style="25" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="21.140625" style="25" bestFit="1" customWidth="1"/>
+    <col min="26" max="16384" width="9.078125" style="25" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
       <c r="A1" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="B1" t="s">
-        <v>78</v>
+        <v>93</v>
       </c>
       <c r="C1" t="s">
-        <v>25</v>
+        <v>27</v>
       </c>
       <c r="D1" t="s">
-        <v>92</v>
+        <v>106</v>
       </c>
       <c r="E1" t="s">
-        <v>98</v>
+        <v>112</v>
       </c>
       <c r="F1" t="s">
-        <v>60</v>
+        <v>69</v>
       </c>
       <c r="G1" t="s">
-        <v>26</v>
+        <v>28</v>
       </c>
       <c r="H1" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="I1" t="s">
-        <v>61</v>
+        <v>16</v>
       </c>
       <c r="J1" t="s">
+        <v>70</v>
+      </c>
+      <c r="K1" t="s">
+        <v>33</v>
+      </c>
+      <c r="L1" t="s">
+        <v>107</v>
+      </c>
+      <c r="M1" t="s">
         <v>34</v>
       </c>
-      <c r="K1" t="s">
-        <v>93</v>
-      </c>
-      <c r="L1" t="s">
-        <v>7</v>
-      </c>
-      <c r="M1" t="s">
-        <v>3</v>
-      </c>
       <c r="N1" t="s">
-        <v>8</v>
+        <v>35</v>
       </c>
       <c r="O1" t="s">
+        <v>36</v>
+      </c>
+      <c r="P1" t="s">
+        <v>51</v>
+      </c>
+      <c r="Q1" t="s">
+        <v>37</v>
+      </c>
+      <c r="R1" t="s">
+        <v>64</v>
+      </c>
+      <c r="S1" t="s">
+        <v>133</v>
+      </c>
+      <c r="T1" t="s">
+        <v>102</v>
+      </c>
+      <c r="U1" t="s">
+        <v>9</v>
+      </c>
+      <c r="V1" t="s">
+        <v>72</v>
+      </c>
+      <c r="W1" t="s">
         <v>45</v>
       </c>
-      <c r="P1" t="s">
-        <v>80</v>
-      </c>
-      <c r="Q1" t="s">
-        <v>107</v>
-      </c>
-      <c r="R1" t="s">
-        <v>16</v>
-      </c>
-      <c r="S1" t="s">
-        <v>46</v>
-      </c>
-      <c r="T1" t="s">
+      <c r="X1" t="s">
+        <v>52</v>
+      </c>
+      <c r="Y1" t="s">
+        <v>134</v>
+      </c>
+    </row>
+    <row r="2" ht="209.05">
+      <c r="A2" s="4" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="6" t="s">
         <v>81</v>
       </c>
-      <c r="U1" t="s">
-        <v>108</v>
-      </c>
-      <c r="V1" t="s">
+      <c r="C2" s="7" t="s">
+        <v>82</v>
+      </c>
+      <c r="D2" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>62</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>83</v>
+      </c>
+      <c r="G2" s="7">
+        <v>30603</v>
+      </c>
+      <c r="H2" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="I2" s="7" t="s">
         <v>17</v>
       </c>
+      <c r="J2" s="4" t="s">
+        <v>4</v>
+      </c>
+      <c r="K2" s="12" t="s">
+        <v>63</v>
+      </c>
+      <c r="L2" s="4" t="s">
+        <v>113</v>
+      </c>
+      <c r="M2" s="4" t="s">
+        <v>84</v>
+      </c>
+      <c r="N2" s="4">
+        <v>82329788</v>
+      </c>
+      <c r="O2" s="12">
+        <v>1</v>
+      </c>
+      <c r="P2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="Q2" s="20" t="s">
+        <v>71</v>
+      </c>
+      <c r="R2" s="4" t="s">
+        <v>5</v>
+      </c>
+      <c r="S2" s="4" t="s">
+        <v>43</v>
+      </c>
+      <c r="T2" s="4" t="s">
+        <v>44</v>
+      </c>
+      <c r="U2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="V2" s="16">
+        <v>44562</v>
+      </c>
+      <c r="W2" s="16">
+        <v>48214</v>
+      </c>
+      <c r="X2" s="4">
+        <v>0</v>
+      </c>
+      <c r="Y2" s="29" t="s">
+        <v>123</v>
+      </c>
     </row>
-    <row r="2" ht="68.8">
-      <c r="A2" s="2" t="s">
-        <v>14</v>
-      </c>
-      <c r="B2" s="2" t="s">
-        <v>6</v>
-      </c>
-      <c r="C2" s="2" t="s">
-        <v>33</v>
-      </c>
-      <c r="D2" s="4" t="s">
-        <v>79</v>
-      </c>
-      <c r="E2" s="4" t="s">
-        <v>59</v>
-      </c>
-      <c r="F2" s="4" t="s">
-        <v>44</v>
-      </c>
-      <c r="G2" s="4">
-        <v>32382</v>
-      </c>
-      <c r="H2" s="4" t="s">
-        <v>106</v>
-      </c>
-      <c r="I2" s="2" t="s">
-        <v>54</v>
-      </c>
-      <c r="J2" s="22" t="s">
-        <v>27</v>
-      </c>
-      <c r="K2" s="2" t="s">
-        <v>88</v>
-      </c>
-      <c r="L2" s="2" t="s">
-        <v>15</v>
-      </c>
-      <c r="M2" s="19">
-        <v>44930</v>
-      </c>
-      <c r="N2" s="23" t="s">
-        <v>28</v>
-      </c>
-      <c r="O2" s="4"/>
-      <c r="P2" s="12"/>
-      <c r="Q2" s="5"/>
-      <c r="R2" s="5"/>
-      <c r="S2" s="5"/>
-      <c r="T2" s="5"/>
-      <c r="U2" s="5"/>
-      <c r="V2" s="20"/>
-    </row>
-    <row r="3">
-      <c r="A3" s="2"/>
-      <c r="B3" s="2"/>
-      <c r="C3" s="2"/>
-      <c r="D3" s="4"/>
-      <c r="E3" s="4"/>
-      <c r="F3" s="4"/>
-      <c r="G3" s="4"/>
-      <c r="H3" s="4"/>
-      <c r="I3" s="2"/>
-      <c r="J3" s="22"/>
-      <c r="K3" s="2"/>
-      <c r="L3" s="2"/>
+    <row r="3" ht="15">
+      <c r="A3" s="4"/>
+      <c r="B3" s="8"/>
+      <c r="C3" s="23"/>
+      <c r="D3" s="8"/>
+      <c r="E3" s="8"/>
+      <c r="F3" s="17"/>
+      <c r="G3" s="7"/>
+      <c r="H3" s="7"/>
+      <c r="I3" s="7"/>
+      <c r="J3" s="4"/>
+      <c r="K3" s="12"/>
+      <c r="L3" s="4"/>
       <c r="M3" s="4"/>
-      <c r="N3" s="2"/>
-      <c r="O3" s="4"/>
-      <c r="P3" s="12"/>
-      <c r="Q3" s="5"/>
-      <c r="R3" s="5"/>
-      <c r="S3" s="5"/>
-      <c r="T3" s="5"/>
+      <c r="N3" s="4"/>
+      <c r="O3" s="2"/>
+      <c r="P3" s="2"/>
+      <c r="Q3" s="2"/>
+      <c r="R3" s="2"/>
+      <c r="S3" s="2"/>
+      <c r="T3" s="2"/>
       <c r="U3" s="2"/>
-      <c r="V3" s="18"/>
+      <c r="V3" s="2"/>
+      <c r="W3" s="2"/>
+      <c r="X3" s="2"/>
+      <c r="Y3" s="18"/>
     </row>
     <row r="4" ht="15">
       <c r="A4" s="2"/>
       <c r="B4" s="2"/>
-      <c r="C4" s="2"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="4"/>
-      <c r="G4" s="4"/>
-      <c r="H4" s="4"/>
+      <c r="C4" s="22"/>
+      <c r="D4" s="2"/>
+      <c r="E4" s="2"/>
+      <c r="F4" s="17"/>
+      <c r="G4" s="2"/>
+      <c r="H4" s="2"/>
       <c r="I4" s="2"/>
-      <c r="J4" s="22"/>
+      <c r="J4" s="2"/>
       <c r="K4" s="2"/>
       <c r="L4" s="2"/>
-      <c r="M4" s="4"/>
-      <c r="N4" s="5"/>
-      <c r="O4" s="4"/>
-      <c r="P4" s="12"/>
-      <c r="Q4" s="5"/>
-      <c r="R4" s="5"/>
-      <c r="S4" s="5"/>
-      <c r="T4" s="5"/>
+      <c r="M4" s="2"/>
+      <c r="N4" s="2"/>
+      <c r="O4" s="2"/>
+      <c r="P4" s="2"/>
+      <c r="Q4" s="2"/>
+      <c r="R4" s="2"/>
+      <c r="S4" s="2"/>
+      <c r="T4" s="2"/>
       <c r="U4" s="2"/>
-      <c r="V4" s="18"/>
-    </row>
-    <row r="5" ht="15">
-      <c r="A5" s="2"/>
-      <c r="B5" s="2"/>
-      <c r="C5" s="2"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="4"/>
-      <c r="G5" s="4"/>
-      <c r="H5" s="4"/>
-      <c r="I5" s="2"/>
-      <c r="J5" s="22"/>
-      <c r="K5" s="2"/>
-      <c r="L5" s="2"/>
-      <c r="M5" s="4"/>
-      <c r="N5" s="4"/>
-      <c r="O5" s="4"/>
-      <c r="P5" s="12"/>
-      <c r="Q5" s="5"/>
-      <c r="R5" s="5"/>
-      <c r="S5" s="5"/>
-      <c r="T5" s="5"/>
-      <c r="U5" s="2"/>
-      <c r="V5" s="18"/>
-    </row>
-    <row r="6" ht="15">
-      <c r="A6" s="2"/>
-      <c r="B6" s="13"/>
-      <c r="C6" s="2"/>
-      <c r="D6" s="2"/>
-      <c r="E6" s="2"/>
-      <c r="F6" s="2"/>
-      <c r="G6" s="7"/>
-      <c r="H6" s="7"/>
-      <c r="I6" s="2"/>
-      <c r="J6" s="2"/>
-      <c r="K6" s="2"/>
-      <c r="L6" s="2"/>
-      <c r="M6" s="2"/>
-      <c r="N6" s="2"/>
-      <c r="O6" s="2"/>
-      <c r="P6" s="2"/>
-      <c r="Q6" s="2"/>
-      <c r="R6" s="2"/>
-      <c r="S6" s="2"/>
-      <c r="T6" s="2"/>
-      <c r="U6" s="2"/>
-      <c r="V6" s="18"/>
-    </row>
-    <row r="7" ht="15">
-      <c r="A7" s="2"/>
-      <c r="B7" s="13"/>
-      <c r="C7" s="2"/>
-      <c r="D7" s="2"/>
-      <c r="E7" s="2"/>
-      <c r="F7" s="2"/>
-      <c r="G7" s="7"/>
-      <c r="H7" s="7"/>
-      <c r="I7" s="2"/>
-      <c r="J7" s="2"/>
-      <c r="K7" s="2"/>
-      <c r="L7" s="2"/>
-      <c r="M7" s="2"/>
-      <c r="N7" s="2"/>
-      <c r="O7" s="2"/>
-      <c r="P7" s="2"/>
-      <c r="Q7" s="2"/>
-      <c r="R7" s="2"/>
-      <c r="S7" s="2"/>
-      <c r="T7" s="2"/>
-      <c r="U7" s="2"/>
-      <c r="V7" s="18"/>
+      <c r="V4" s="2"/>
+      <c r="W4" s="2"/>
+      <c r="X4" s="2"/>
+      <c r="Y4" s="18"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1466,7 +1532,7 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="16384" width="9.078125" style="10" customWidth="1"/>
+    <col min="1" max="16384" width="9.078125" style="14" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1"/>
@@ -1485,214 +1551,214 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15.1"/>
   <cols>
-    <col min="1" max="1" width="9.078125" style="16" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="14.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="33.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="25.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="31.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="26.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="8" max="8" width="12.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="9" max="9" width="18.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="10" max="11" width="12.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="12" max="12" width="57.140625" style="16" customWidth="1"/>
-    <col min="13" max="14" width="61" style="16" customWidth="1"/>
-    <col min="15" max="15" width="47" style="16" bestFit="1" customWidth="1"/>
-    <col min="16" max="16" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="17" max="17" width="103.7109375" style="16" bestFit="1" customWidth="1"/>
-    <col min="18" max="18" width="69.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="19" max="20" width="61" style="16" bestFit="1" customWidth="1"/>
-    <col min="21" max="21" width="63.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="22" max="22" width="15.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="23" max="23" width="10.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="24" max="24" width="15.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="25" max="25" width="15.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="26" max="26" width="51" style="16" bestFit="1" customWidth="1"/>
-    <col min="27" max="27" width="49.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="28" max="28" width="59.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="29" max="29" width="49.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="30" max="30" width="53.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="31" max="31" width="56.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="32" max="32" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="33" max="33" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="34" max="34" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="35" max="36" width="62.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="37" max="37" width="51.28515625" style="16" bestFit="1" customWidth="1"/>
-    <col min="38" max="38" width="57.42578125" style="16" bestFit="1" customWidth="1"/>
-    <col min="39" max="39" width="57.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="40" max="40" width="53.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="41" max="41" width="35.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="42" max="42" width="58.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="43" max="43" width="17.5703125" style="16" bestFit="1" customWidth="1"/>
-    <col min="44" max="44" width="12.85546875" style="16" bestFit="1" customWidth="1"/>
-    <col min="45" max="45" width="19.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="46" max="46" width="21.140625" style="16" bestFit="1" customWidth="1"/>
-    <col min="47" max="16384" width="9.078125" style="16" customWidth="1"/>
+    <col min="1" max="1" width="9.078125" style="28" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="14.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="33.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="25.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="31.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="26.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="8" max="8" width="12.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="9" max="9" width="18.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="10" max="11" width="12.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="12" max="12" width="57.140625" style="28" customWidth="1"/>
+    <col min="13" max="14" width="61" style="28" customWidth="1"/>
+    <col min="15" max="15" width="47" style="28" bestFit="1" customWidth="1"/>
+    <col min="16" max="16" width="63.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="17" max="17" width="103.7109375" style="28" bestFit="1" customWidth="1"/>
+    <col min="18" max="18" width="69.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="19" max="20" width="61" style="28" bestFit="1" customWidth="1"/>
+    <col min="21" max="21" width="63.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="22" max="22" width="15.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="23" max="23" width="10.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="24" max="24" width="15.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="25" max="25" width="15.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="26" max="26" width="51" style="28" bestFit="1" customWidth="1"/>
+    <col min="27" max="27" width="49.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="28" max="28" width="59.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="29" max="29" width="49.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="30" max="30" width="53.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="31" max="31" width="56.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="32" max="32" width="57.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="33" max="33" width="53.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="34" max="34" width="58.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="35" max="36" width="62.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="37" max="37" width="51.28515625" style="28" bestFit="1" customWidth="1"/>
+    <col min="38" max="38" width="57.42578125" style="28" bestFit="1" customWidth="1"/>
+    <col min="39" max="39" width="57.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="40" max="40" width="53.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="41" max="41" width="35.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="42" max="42" width="58.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="43" max="43" width="17.5703125" style="28" bestFit="1" customWidth="1"/>
+    <col min="44" max="44" width="12.85546875" style="28" bestFit="1" customWidth="1"/>
+    <col min="45" max="45" width="19.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="46" max="46" width="21.140625" style="28" bestFit="1" customWidth="1"/>
+    <col min="47" max="16384" width="9.078125" style="28" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" customFormat="1">
       <c r="A1" t="s">
-        <v>39</v>
+        <v>46</v>
       </c>
       <c r="B1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="C1" t="s">
-        <v>116</v>
+        <v>135</v>
       </c>
       <c r="D1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="E1" t="s">
-        <v>47</v>
+        <v>53</v>
       </c>
       <c r="F1" t="s">
-        <v>82</v>
+        <v>94</v>
       </c>
       <c r="G1" t="s">
         <v>29</v>
       </c>
       <c r="H1" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
       <c r="I1" t="s">
-        <v>70</v>
+        <v>85</v>
       </c>
       <c r="J1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="K1" t="s">
-        <v>64</v>
+        <v>75</v>
       </c>
       <c r="L1" t="s">
-        <v>71</v>
+        <v>86</v>
       </c>
       <c r="M1" t="s">
-        <v>99</v>
+        <v>114</v>
       </c>
       <c r="N1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="O1" t="s">
-        <v>45</v>
+        <v>54</v>
       </c>
       <c r="P1" t="s">
-        <v>80</v>
+        <v>95</v>
       </c>
       <c r="Q1" t="s">
-        <v>107</v>
+        <v>125</v>
       </c>
       <c r="R1" t="s">
-        <v>16</v>
+        <v>18</v>
       </c>
       <c r="S1" t="s">
-        <v>46</v>
+        <v>55</v>
       </c>
       <c r="T1" t="s">
-        <v>81</v>
+        <v>96</v>
       </c>
       <c r="U1" t="s">
-        <v>108</v>
+        <v>126</v>
       </c>
       <c r="V1" t="s">
-        <v>17</v>
+        <v>22</v>
       </c>
       <c r="W1" t="s">
-        <v>55</v>
+        <v>65</v>
       </c>
       <c r="X1" t="s">
-        <v>89</v>
+        <v>103</v>
       </c>
       <c r="Y1" t="s">
-        <v>117</v>
+        <v>136</v>
       </c>
       <c r="Z1" t="s">
         <v>30</v>
       </c>
       <c r="AA1" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="AB1" t="s">
-        <v>65</v>
+        <v>76</v>
       </c>
       <c r="AC1" t="s">
-        <v>94</v>
+        <v>108</v>
       </c>
       <c r="AD1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="AE1" t="s">
-        <v>40</v>
+        <v>47</v>
       </c>
       <c r="AF1" t="s">
-        <v>72</v>
+        <v>87</v>
       </c>
       <c r="AG1" t="s">
-        <v>100</v>
+        <v>115</v>
       </c>
       <c r="AH1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="AI1" t="s">
-        <v>41</v>
+        <v>48</v>
       </c>
       <c r="AJ1" t="s">
-        <v>73</v>
+        <v>88</v>
       </c>
       <c r="AK1" t="s">
-        <v>101</v>
+        <v>116</v>
       </c>
       <c r="AL1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="AM1" t="s">
-        <v>48</v>
+        <v>56</v>
       </c>
       <c r="AN1" t="s">
-        <v>83</v>
+        <v>97</v>
       </c>
       <c r="AO1" t="s">
-        <v>110</v>
+        <v>127</v>
       </c>
       <c r="AP1" t="s">
-        <v>21</v>
+        <v>23</v>
       </c>
       <c r="AQ1" t="s">
-        <v>49</v>
+        <v>57</v>
       </c>
       <c r="AR1" t="s">
-        <v>84</v>
+        <v>98</v>
       </c>
       <c r="AS1" t="s">
-        <v>111</v>
+        <v>128</v>
       </c>
       <c r="AT1" t="s">
-        <v>22</v>
+        <v>24</v>
       </c>
     </row>
     <row r="2" ht="36">
-      <c r="A2" s="7" t="s">
-        <v>62</v>
-      </c>
-      <c r="B2" s="7" t="s">
-        <v>109</v>
-      </c>
-      <c r="C2" s="25">
+      <c r="A2" s="15" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="15" t="s">
+        <v>124</v>
+      </c>
+      <c r="C2" s="24">
         <v>192168132154</v>
       </c>
-      <c r="D2" s="4" t="str">
+      <c r="D2" s="10" t="str">
         <f>"Verifikasi Database "&amp;J2</f>
         <v>Verifikasi Database DPLK</v>
       </c>
-      <c r="E2" s="4"/>
-      <c r="F2" s="15"/>
-      <c r="G2" s="9" t="s">
-        <v>63</v>
-      </c>
-      <c r="H2" s="9"/>
+      <c r="E2" s="10"/>
+      <c r="F2" s="27"/>
+      <c r="G2" s="13" t="s">
+        <v>74</v>
+      </c>
+      <c r="H2" s="13"/>
       <c r="I2" s="2"/>
       <c r="J2" s="2" t="s">
-        <v>23</v>
+        <v>25</v>
       </c>
       <c r="K2" s="2"/>
       <c r="L2" s="1"/>
@@ -1705,7 +1771,7 @@
       <c r="S2" s="1"/>
       <c r="T2" s="1"/>
       <c r="U2" s="1"/>
-      <c r="V2" s="17"/>
+      <c r="V2" s="21"/>
       <c r="W2" s="1"/>
       <c r="X2" s="1"/>
       <c r="Y2" s="1"/>
@@ -1726,10 +1792,10 @@
       <c r="AN2" s="1"/>
       <c r="AO2" s="1"/>
       <c r="AP2" s="1"/>
-      <c r="AQ2" s="8"/>
-      <c r="AR2" s="8"/>
-      <c r="AS2" s="8"/>
-      <c r="AT2" s="24"/>
+      <c r="AQ2" s="9"/>
+      <c r="AR2" s="9"/>
+      <c r="AS2" s="9"/>
+      <c r="AT2" s="19"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>